<commit_message>
version 1 of excelparse.js
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,25 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakewood\Develop\ALCOASSR\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9495"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -41,14 +31,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -355,11 +345,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
the modified data now spawns a new column to the left
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Parcelld</t>
   </si>
@@ -22,10 +22,19 @@
     <t>078C-0415-006-00</t>
   </si>
   <si>
+    <t>078C041500600</t>
+  </si>
+  <si>
     <t>078C-0445-036-00</t>
   </si>
   <si>
+    <t>078C044503600</t>
+  </si>
+  <si>
     <t>234G-9345-034-00</t>
+  </si>
+  <si>
+    <t>234G934503400</t>
   </si>
 </sst>
 </file>
@@ -343,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
@@ -354,24 +363,36 @@
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more verbosity to excel parse
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9495"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Parcelld</t>
   </si>
@@ -22,23 +22,32 @@
     <t>078C-0415-006-00</t>
   </si>
   <si>
+    <t>078C041500600</t>
+  </si>
+  <si>
     <t>078C-0445-036-00</t>
   </si>
   <si>
+    <t>078C044503600</t>
+  </si>
+  <si>
     <t>234G-9345-034-00</t>
+  </si>
+  <si>
+    <t>234G934503400</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -343,35 +352,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New pdf example, and changed column processing
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -352,46 +352,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="R1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="R2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="R3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="R4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>